<commit_message>
Halfway through removing multiple excelsheets
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/orderFullFillmentFlow.xlsx
+++ b/resources/ExcelsheetData/orderFullFillmentFlow.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="RegistrationErrorScenarios" localSheetId="0">Sheet1!$B$1:$C$2</definedName>
+    <definedName name="RegistrationErrorScenarios" localSheetId="0">Sheet1!$B$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>password</t>
   </si>
@@ -75,39 +75,18 @@
     <t>TC_OrderFullFillmentFlow_004</t>
   </si>
   <si>
-    <t>TC_OrderFullFillmentFlow_005</t>
-  </si>
-  <si>
-    <t>TC_OrderFullFillmentFlow_006</t>
-  </si>
-  <si>
     <t>emailId</t>
   </si>
   <si>
     <t>hemanth.bs123@unilogcorp.com</t>
   </si>
   <si>
-    <t>'hemanth.bs123@unilogcorp.com</t>
-  </si>
-  <si>
     <t>searchText</t>
   </si>
   <si>
     <t>phoneNumber</t>
   </si>
   <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>1234567891</t>
-  </si>
-  <si>
-    <t>1234567892</t>
-  </si>
-  <si>
-    <t>1234567893</t>
-  </si>
-  <si>
     <t>1234567894</t>
   </si>
   <si>
@@ -129,15 +108,6 @@
     <t>12345</t>
   </si>
   <si>
-    <t>12346</t>
-  </si>
-  <si>
-    <t>12347</t>
-  </si>
-  <si>
-    <t>12348</t>
-  </si>
-  <si>
     <t>12349</t>
   </si>
   <si>
@@ -159,13 +129,25 @@
     <t>Testing from Unilog, Please do not process.</t>
   </si>
   <si>
+    <t>Ordered By</t>
+  </si>
+  <si>
     <t>hemanth.bs@unilogcorp.com</t>
   </si>
   <si>
-    <t>Ordered By</t>
-  </si>
-  <si>
-    <t>Hemanth</t>
+    <t>Hemanth BS</t>
+  </si>
+  <si>
+    <t>UPS Ground</t>
+  </si>
+  <si>
+    <t>UPS 1 DAY</t>
+  </si>
+  <si>
+    <t>OT OUR TRUCK</t>
+  </si>
+  <si>
+    <t>PICK UP</t>
   </si>
 </sst>
 </file>
@@ -189,9 +171,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -241,11 +222,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -259,18 +239,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -553,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,8 +552,9 @@
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
     <col min="9" max="9" width="33.42578125" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
     <col min="11" max="11" width="47.140625" customWidth="1"/>
@@ -580,258 +567,210 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>33</v>
+      <c r="M2" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="7" t="s">
-        <v>35</v>
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="7" t="s">
-        <v>35</v>
+      <c r="I5" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="hemanthsridhar92@gmail.com"/>
-    <hyperlink ref="I3:I7" r:id="rId2" display="hemanth.bs@unilogcorp.com"/>
+    <hyperlink ref="B2:B5" r:id="rId1" display="hemanth.bs123@unilogcorp.com"/>
+    <hyperlink ref="I2:I5" r:id="rId2" display="hemanth.bs@unilogcorp.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>